<commit_message>
Fix market regime analyzer by reverting to original predictor
Root cause: ML emergency fix had switched to market_regime_predictor_fixed which lacked:
- update_actual_regime() method
- get_model_insights() method

Solution: Reverted to using original market_regime_predictor.py which has all required methods
Now displays model performance (90.9% accuracy) in dashboard insights
</commit_message>
<xml_diff>
--- a/Daily/data/short_momentum/latest_short_momentum.xlsx
+++ b/Daily/data/short_momentum/latest_short_momentum.xlsx
@@ -64,276 +64,276 @@
     <t>AUBANK</t>
   </si>
   <si>
+    <t>MGL</t>
+  </si>
+  <si>
+    <t>AUROPHARMA</t>
+  </si>
+  <si>
+    <t>POWERGRID</t>
+  </si>
+  <si>
+    <t>CHOLAFIN</t>
+  </si>
+  <si>
     <t>TATATECH</t>
   </si>
   <si>
-    <t>AUROPHARMA</t>
-  </si>
-  <si>
-    <t>CHOLAFIN</t>
-  </si>
-  <si>
-    <t>MGL</t>
-  </si>
-  <si>
-    <t>POWERGRID</t>
+    <t>SPARC</t>
+  </si>
+  <si>
+    <t>GUJGASLTD</t>
   </si>
   <si>
     <t>INOXWIND</t>
   </si>
   <si>
-    <t>GUJGASLTD</t>
-  </si>
-  <si>
-    <t>SPARC</t>
+    <t>JUBLFOOD</t>
   </si>
   <si>
     <t>ICICIPRULI</t>
   </si>
   <si>
+    <t>HAPPSTMNDS</t>
+  </si>
+  <si>
+    <t>AARTIIND</t>
+  </si>
+  <si>
     <t>IIFL</t>
   </si>
   <si>
-    <t>HAPPSTMNDS</t>
-  </si>
-  <si>
     <t>IRB</t>
   </si>
   <si>
-    <t>AARTIIND</t>
-  </si>
-  <si>
     <t>SHRIRAMFIN</t>
   </si>
   <si>
-    <t>JUBLFOOD</t>
-  </si>
-  <si>
     <t>HFCL</t>
   </si>
   <si>
+    <t>IREDA</t>
+  </si>
+  <si>
+    <t>RECLTD</t>
+  </si>
+  <si>
+    <t>BAJAJ-AUTO</t>
+  </si>
+  <si>
+    <t>APLLTD</t>
+  </si>
+  <si>
+    <t>BHARTIARTL</t>
+  </si>
+  <si>
+    <t>POONAWALLA</t>
+  </si>
+  <si>
+    <t>ADANIGREEN</t>
+  </si>
+  <si>
+    <t>TRITURBINE</t>
+  </si>
+  <si>
+    <t>M&amp;MFIN</t>
+  </si>
+  <si>
     <t>AVG</t>
   </si>
   <si>
-    <t>RECLTD</t>
-  </si>
-  <si>
-    <t>APLLTD</t>
-  </si>
-  <si>
-    <t>BAJAJ-AUTO</t>
-  </si>
-  <si>
-    <t>POONAWALLA</t>
+    <t>BIOCON</t>
+  </si>
+  <si>
+    <t>TATACONSUM</t>
+  </si>
+  <si>
+    <t>RAYMOND</t>
+  </si>
+  <si>
+    <t>CELLO</t>
+  </si>
+  <si>
+    <t>EQUITASBNK</t>
+  </si>
+  <si>
+    <t>RVNL</t>
+  </si>
+  <si>
+    <t>SUNTV</t>
+  </si>
+  <si>
+    <t>LATENTVIEW</t>
+  </si>
+  <si>
+    <t>KEC</t>
+  </si>
+  <si>
+    <t>IRCTC</t>
   </si>
   <si>
     <t>IOC</t>
   </si>
   <si>
-    <t>ADANIGREEN</t>
-  </si>
-  <si>
-    <t>KEC</t>
-  </si>
-  <si>
-    <t>CELLO</t>
-  </si>
-  <si>
-    <t>BIOCON</t>
-  </si>
-  <si>
-    <t>RVNL</t>
-  </si>
-  <si>
-    <t>EQUITASBNK</t>
-  </si>
-  <si>
-    <t>TATACONSUM</t>
-  </si>
-  <si>
-    <t>BHARTIARTL</t>
-  </si>
-  <si>
-    <t>IREDA</t>
-  </si>
-  <si>
-    <t>M&amp;MFIN</t>
+    <t>CAMPUS</t>
+  </si>
+  <si>
+    <t>ANGELONE</t>
+  </si>
+  <si>
+    <t>AZAD</t>
+  </si>
+  <si>
+    <t>THERMAX</t>
+  </si>
+  <si>
+    <t>ABBOTINDIA</t>
+  </si>
+  <si>
+    <t>MAHLIFE</t>
+  </si>
+  <si>
+    <t>SBICARD</t>
+  </si>
+  <si>
+    <t>NESTLEIND</t>
+  </si>
+  <si>
+    <t>HDFCLIFE</t>
+  </si>
+  <si>
+    <t>ADANIENT</t>
+  </si>
+  <si>
+    <t>RENUKA</t>
+  </si>
+  <si>
+    <t>CHENNPETRO</t>
+  </si>
+  <si>
+    <t>BAJAJFINSV</t>
+  </si>
+  <si>
+    <t>KALYANKJIL</t>
+  </si>
+  <si>
+    <t>SKFINDIA</t>
+  </si>
+  <si>
+    <t>TANLA</t>
+  </si>
+  <si>
+    <t>RBLBANK</t>
+  </si>
+  <si>
+    <t>AAVAS</t>
+  </si>
+  <si>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>PDSL</t>
+  </si>
+  <si>
+    <t>AIAENG</t>
+  </si>
+  <si>
+    <t>MAITHANALL</t>
+  </si>
+  <si>
+    <t>PAGEIND</t>
+  </si>
+  <si>
+    <t>MMTC</t>
+  </si>
+  <si>
+    <t>JKLAKSHMI</t>
+  </si>
+  <si>
+    <t>ALEMBICLTD</t>
+  </si>
+  <si>
+    <t>TMB</t>
+  </si>
+  <si>
+    <t>DLF</t>
+  </si>
+  <si>
+    <t>ICICIBANK</t>
   </si>
   <si>
     <t>SMSPHARMA</t>
   </si>
   <si>
-    <t>SUNTV</t>
-  </si>
-  <si>
-    <t>CAMPUS</t>
-  </si>
-  <si>
-    <t>ABBOTINDIA</t>
-  </si>
-  <si>
-    <t>RAYMOND</t>
-  </si>
-  <si>
-    <t>IRCTC</t>
-  </si>
-  <si>
-    <t>ANGELONE</t>
-  </si>
-  <si>
-    <t>AAVAS</t>
-  </si>
-  <si>
-    <t>THERMAX</t>
-  </si>
-  <si>
-    <t>MAHLIFE</t>
-  </si>
-  <si>
-    <t>ADANIENT</t>
-  </si>
-  <si>
-    <t>SKFINDIA</t>
-  </si>
-  <si>
-    <t>HDFCLIFE</t>
-  </si>
-  <si>
-    <t>CHENNPETRO</t>
-  </si>
-  <si>
-    <t>BAJAJFINSV</t>
-  </si>
-  <si>
-    <t>AZAD</t>
-  </si>
-  <si>
-    <t>LATENTVIEW</t>
-  </si>
-  <si>
-    <t>TMB</t>
-  </si>
-  <si>
-    <t>TANLA</t>
-  </si>
-  <si>
-    <t>NESTLEIND</t>
-  </si>
-  <si>
-    <t>KALYANKJIL</t>
-  </si>
-  <si>
-    <t>AIAENG</t>
-  </si>
-  <si>
-    <t>PAGEIND</t>
-  </si>
-  <si>
-    <t>MAITHANALL</t>
-  </si>
-  <si>
-    <t>TRITURBINE</t>
-  </si>
-  <si>
-    <t>SANOFI</t>
-  </si>
-  <si>
-    <t>RBLBANK</t>
-  </si>
-  <si>
-    <t>DLF</t>
-  </si>
-  <si>
-    <t>JKLAKSHMI</t>
-  </si>
-  <si>
-    <t>MMTC</t>
-  </si>
-  <si>
-    <t>ALEMBICLTD</t>
-  </si>
-  <si>
     <t>BPCL</t>
   </si>
   <si>
+    <t>DABUR</t>
+  </si>
+  <si>
     <t>HCLTECH</t>
   </si>
   <si>
-    <t>PDSL</t>
-  </si>
-  <si>
-    <t>RENUKA</t>
+    <t>BATAINDIA</t>
+  </si>
+  <si>
+    <t>ANURAS</t>
+  </si>
+  <si>
+    <t>AWL</t>
+  </si>
+  <si>
+    <t>HDFCBANK</t>
+  </si>
+  <si>
+    <t>ASTRAZEN</t>
+  </si>
+  <si>
+    <t>NATCOPHARM</t>
   </si>
   <si>
     <t>JINDALSAW</t>
   </si>
   <si>
-    <t>ICICIBANK</t>
-  </si>
-  <si>
-    <t>SBICARD</t>
-  </si>
-  <si>
-    <t>NATCOPHARM</t>
+    <t>BSOFT</t>
+  </si>
+  <si>
+    <t>UBL</t>
+  </si>
+  <si>
+    <t>RKFORGE</t>
+  </si>
+  <si>
+    <t>NAUKRI</t>
+  </si>
+  <si>
+    <t>PRSMJOHNSN</t>
+  </si>
+  <si>
+    <t>MVGJL</t>
   </si>
   <si>
     <t>VEDL</t>
   </si>
   <si>
-    <t>PRSMJOHNSN</t>
-  </si>
-  <si>
-    <t>AWL</t>
-  </si>
-  <si>
-    <t>MVGJL</t>
+    <t>GNFC</t>
+  </si>
+  <si>
+    <t>EPACK</t>
   </si>
   <si>
     <t>UJJIVANSFB</t>
   </si>
   <si>
-    <t>DABUR</t>
-  </si>
-  <si>
     <t>WHIRLPOOL</t>
   </si>
   <si>
     <t>EMBDL</t>
   </si>
   <si>
-    <t>ANURAS</t>
-  </si>
-  <si>
-    <t>BSOFT</t>
-  </si>
-  <si>
     <t>RBA</t>
   </si>
   <si>
-    <t>ASTRAZEN</t>
-  </si>
-  <si>
-    <t>GNFC</t>
-  </si>
-  <si>
-    <t>RKFORGE</t>
-  </si>
-  <si>
-    <t>EPACK</t>
-  </si>
-  <si>
-    <t>NAUKRI</t>
-  </si>
-  <si>
-    <t>BATAINDIA</t>
-  </si>
-  <si>
-    <t>UBL</t>
-  </si>
-  <si>
-    <t>HDFCBANK</t>
-  </si>
-  <si>
     <t>Financial Services</t>
   </si>
   <si>
@@ -343,10 +343,13 @@
     <t>Healthcare</t>
   </si>
   <si>
+    <t>Utilities</t>
+  </si>
+  <si>
     <t>Industrials</t>
   </si>
   <si>
-    <t>Utilities</t>
+    <t>Consumer Cyclical</t>
   </si>
   <si>
     <t>Technology</t>
@@ -355,13 +358,10 @@
     <t>Basic Materials</t>
   </si>
   <si>
-    <t>Consumer Cyclical</t>
+    <t>Communication Services</t>
   </si>
   <si>
     <t>Energy</t>
-  </si>
-  <si>
-    <t>Communication Services</t>
   </si>
   <si>
     <t>Real Estate</t>
@@ -807,10 +807,10 @@
         <v>150</v>
       </c>
       <c r="F2">
-        <v>0.83</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="G2">
-        <v>-1.08</v>
+        <v>-1.05</v>
       </c>
       <c r="H2">
         <v>-2.15</v>
@@ -822,10 +822,10 @@
         <v>0.5</v>
       </c>
       <c r="K2">
-        <v>0.05083342525182209</v>
+        <v>0.03433498288401891</v>
       </c>
       <c r="L2">
-        <v>0.1280056026768345</v>
+        <v>0.2299213012231813</v>
       </c>
       <c r="M2" t="s">
         <v>118</v>
@@ -834,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="O2">
-        <v>724.6</v>
+        <v>724.25</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -845,22 +845,22 @@
         <v>107</v>
       </c>
       <c r="C3">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <v>120</v>
       </c>
       <c r="F3">
-        <v>0.19</v>
+        <v>0.44</v>
       </c>
       <c r="G3">
-        <v>-0.46</v>
+        <v>-1.03</v>
       </c>
       <c r="H3">
-        <v>-2.5</v>
+        <v>-0.63</v>
       </c>
       <c r="I3">
         <v>50</v>
@@ -869,10 +869,10 @@
         <v>0.5</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>0.2701713899755208</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>0.6310599835661462</v>
       </c>
       <c r="M3" t="s">
         <v>119</v>
@@ -881,7 +881,7 @@
         <v>12</v>
       </c>
       <c r="O3">
-        <v>663.95</v>
+        <v>1262.5</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -901,10 +901,10 @@
         <v>140</v>
       </c>
       <c r="F4">
-        <v>0.67</v>
+        <v>0.89</v>
       </c>
       <c r="G4">
-        <v>-0.11</v>
+        <v>-0.04</v>
       </c>
       <c r="H4">
         <v>0.57</v>
@@ -916,10 +916,10 @@
         <v>0.5</v>
       </c>
       <c r="K4">
-        <v>0.109490262002456</v>
+        <v>0.007205656978457615</v>
       </c>
       <c r="L4">
-        <v>0.2147427786414085</v>
+        <v>0.06706706706706707</v>
       </c>
       <c r="M4" t="s">
         <v>120</v>
@@ -928,7 +928,7 @@
         <v>14</v>
       </c>
       <c r="O4">
-        <v>1030.6</v>
+        <v>1030.9</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -936,25 +936,25 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5">
         <v>160</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="F5">
-        <v>1.25</v>
+        <v>1.12</v>
       </c>
       <c r="G5">
-        <v>-0.32</v>
+        <v>-0.33</v>
       </c>
       <c r="H5">
-        <v>-2.47</v>
+        <v>-1.95</v>
       </c>
       <c r="I5">
         <v>50</v>
@@ -963,19 +963,19 @@
         <v>0.5</v>
       </c>
       <c r="K5">
-        <v>0.3300103844866635</v>
+        <v>0.02239833551706121</v>
       </c>
       <c r="L5">
-        <v>0.6721440247967221</v>
+        <v>0.05420934459727907</v>
       </c>
       <c r="M5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="O5">
-        <v>1444.9</v>
+        <v>275.55</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -983,25 +983,25 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D6">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="F6">
-        <v>0.05</v>
+        <v>1.06</v>
       </c>
       <c r="G6">
-        <v>-1.21</v>
+        <v>-0.45</v>
       </c>
       <c r="H6">
-        <v>-0.63</v>
+        <v>-2.47</v>
       </c>
       <c r="I6">
         <v>50</v>
@@ -1010,19 +1010,19 @@
         <v>0.5</v>
       </c>
       <c r="K6">
-        <v>0.5567574446424134</v>
+        <v>0.2968549387238579</v>
       </c>
       <c r="L6">
-        <v>0.5680895958448303</v>
+        <v>0.628769979152189</v>
       </c>
       <c r="M6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O6">
-        <v>1259.3</v>
+        <v>1443.5</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1036,19 +1036,19 @@
         <v>150</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E7">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="F7">
-        <v>0.86</v>
+        <v>0.25</v>
       </c>
       <c r="G7">
-        <v>-0.52</v>
+        <v>-0.6</v>
       </c>
       <c r="H7">
-        <v>-1.95</v>
+        <v>-2.5</v>
       </c>
       <c r="I7">
         <v>50</v>
@@ -1057,19 +1057,19 @@
         <v>0.5</v>
       </c>
       <c r="K7">
-        <v>1.415049487431057</v>
+        <v>0.8554017882568019</v>
       </c>
       <c r="L7">
-        <v>3.33467210074554</v>
+        <v>1.147528459011383</v>
       </c>
       <c r="M7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O7">
-        <v>274.95</v>
+        <v>664</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1077,7 +1077,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8">
         <v>140</v>
@@ -1089,13 +1089,13 @@
         <v>120</v>
       </c>
       <c r="F8">
-        <v>0.71</v>
+        <v>0.62</v>
       </c>
       <c r="G8">
-        <v>0.89</v>
+        <v>0.2</v>
       </c>
       <c r="H8">
-        <v>-0.15</v>
+        <v>-0.32</v>
       </c>
       <c r="I8">
         <v>50</v>
@@ -1104,10 +1104,10 @@
         <v>0.5</v>
       </c>
       <c r="K8">
-        <v>0.06057475774882631</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0.125200096014294</v>
+        <v>0.2660133006650333</v>
       </c>
       <c r="M8" t="s">
         <v>120</v>
@@ -1116,7 +1116,7 @@
         <v>12</v>
       </c>
       <c r="O8">
-        <v>139.3</v>
+        <v>140.8</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1124,7 +1124,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9">
         <v>140</v>
@@ -1136,10 +1136,10 @@
         <v>120</v>
       </c>
       <c r="F9">
-        <v>0.77</v>
+        <v>1.06</v>
       </c>
       <c r="G9">
-        <v>0.19</v>
+        <v>0.04</v>
       </c>
       <c r="H9">
         <v>0.29</v>
@@ -1151,10 +1151,10 @@
         <v>0.5</v>
       </c>
       <c r="K9">
-        <v>0.0049744104845279</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0.03271674845853781</v>
+        <v>0</v>
       </c>
       <c r="M9" t="s">
         <v>120</v>
@@ -1163,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="O9">
-        <v>420.85</v>
+        <v>421</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1171,7 +1171,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C10">
         <v>140</v>
@@ -1183,13 +1183,13 @@
         <v>120</v>
       </c>
       <c r="F10">
-        <v>0.39</v>
+        <v>0.66</v>
       </c>
       <c r="G10">
-        <v>-0.06</v>
+        <v>0.8</v>
       </c>
       <c r="H10">
-        <v>-0.32</v>
+        <v>-0.15</v>
       </c>
       <c r="I10">
         <v>50</v>
@@ -1198,10 +1198,10 @@
         <v>0.5</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>0.05829532727873551</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.233640734230655</v>
       </c>
       <c r="M10" t="s">
         <v>120</v>
@@ -1210,7 +1210,7 @@
         <v>12</v>
       </c>
       <c r="O10">
-        <v>140.55</v>
+        <v>139.43</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1218,25 +1218,25 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C11">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D11">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F11">
-        <v>0.83</v>
+        <v>0.76</v>
       </c>
       <c r="G11">
-        <v>-1.3</v>
+        <v>-0.42</v>
       </c>
       <c r="H11">
-        <v>-1.1</v>
+        <v>-0.82</v>
       </c>
       <c r="I11">
         <v>50</v>
@@ -1245,19 +1245,19 @@
         <v>0.5</v>
       </c>
       <c r="K11">
-        <v>0.01484313867846261</v>
+        <v>0.005198759724461245</v>
       </c>
       <c r="L11">
-        <v>0.07393715341959335</v>
+        <v>0.06729151646238885</v>
       </c>
       <c r="M11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N11">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="O11">
-        <v>605.5</v>
+        <v>633.75</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1268,22 +1268,22 @@
         <v>106</v>
       </c>
       <c r="C12">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D12">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E12">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F12">
-        <v>2.21</v>
+        <v>0.66</v>
       </c>
       <c r="G12">
-        <v>0.07000000000000001</v>
+        <v>-1.7</v>
       </c>
       <c r="H12">
-        <v>-0.48</v>
+        <v>-1.1</v>
       </c>
       <c r="I12">
         <v>50</v>
@@ -1292,19 +1292,19 @@
         <v>0.5</v>
       </c>
       <c r="K12">
-        <v>0.06682945636808009</v>
+        <v>0.3146509341198203</v>
       </c>
       <c r="L12">
-        <v>0.3708199308126479</v>
+        <v>0.5516596540439458</v>
       </c>
       <c r="M12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N12">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O12">
-        <v>437.8</v>
+        <v>605.55</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1312,7 +1312,7 @@
         <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C13">
         <v>130</v>
@@ -1324,10 +1324,10 @@
         <v>110</v>
       </c>
       <c r="F13">
-        <v>0.43</v>
+        <v>0.76</v>
       </c>
       <c r="G13">
-        <v>-0.3</v>
+        <v>-0.11</v>
       </c>
       <c r="H13">
         <v>0.59</v>
@@ -1339,10 +1339,10 @@
         <v>0.5</v>
       </c>
       <c r="K13">
-        <v>0.0005038544868249103</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>0.006329781622534023</v>
+        <v>0</v>
       </c>
       <c r="M13" t="s">
         <v>120</v>
@@ -1351,7 +1351,7 @@
         <v>11</v>
       </c>
       <c r="O13">
-        <v>566.15</v>
+        <v>566.95</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1359,7 +1359,7 @@
         <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C14">
         <v>130</v>
@@ -1371,13 +1371,13 @@
         <v>110</v>
       </c>
       <c r="F14">
-        <v>0.7</v>
+        <v>0.92</v>
       </c>
       <c r="G14">
-        <v>1.4</v>
+        <v>0.29</v>
       </c>
       <c r="H14">
-        <v>0.42</v>
+        <v>-1.31</v>
       </c>
       <c r="I14">
         <v>50</v>
@@ -1386,10 +1386,10 @@
         <v>0.5</v>
       </c>
       <c r="K14">
-        <v>0.3929542967079354</v>
+        <v>0.03349460364719289</v>
       </c>
       <c r="L14">
-        <v>0.6658388763345126</v>
+        <v>0.03772398616787174</v>
       </c>
       <c r="M14" t="s">
         <v>120</v>
@@ -1398,7 +1398,7 @@
         <v>11</v>
       </c>
       <c r="O14">
-        <v>43.4</v>
+        <v>379.65</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1406,7 +1406,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C15">
         <v>130</v>
@@ -1418,13 +1418,13 @@
         <v>110</v>
       </c>
       <c r="F15">
-        <v>0.8100000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="G15">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="H15">
-        <v>-1.31</v>
+        <v>-0.48</v>
       </c>
       <c r="I15">
         <v>50</v>
@@ -1433,10 +1433,10 @@
         <v>0.5</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>0.2164481790974647</v>
       </c>
       <c r="L15">
-        <v>0.04454144581533117</v>
+        <v>0.5479239184485331</v>
       </c>
       <c r="M15" t="s">
         <v>120</v>
@@ -1445,7 +1445,7 @@
         <v>11</v>
       </c>
       <c r="O15">
-        <v>379.55</v>
+        <v>438.55</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1453,25 +1453,25 @@
         <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C16">
         <v>130</v>
       </c>
       <c r="D16">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="F16">
-        <v>0.8100000000000001</v>
+        <v>0.98</v>
       </c>
       <c r="G16">
-        <v>1.66</v>
+        <v>1.43</v>
       </c>
       <c r="H16">
-        <v>-0.66</v>
+        <v>0.42</v>
       </c>
       <c r="I16">
         <v>50</v>
@@ -1480,19 +1480,19 @@
         <v>0.5</v>
       </c>
       <c r="K16">
-        <v>0.3700776706332395</v>
+        <v>0.2679039020132577</v>
       </c>
       <c r="L16">
-        <v>1.690289055813428</v>
+        <v>0.3949687524721145</v>
       </c>
       <c r="M16" t="s">
         <v>120</v>
       </c>
       <c r="N16">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O16">
-        <v>584.6</v>
+        <v>43.4</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1500,25 +1500,25 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C17">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D17">
         <v>20</v>
       </c>
       <c r="E17">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F17">
-        <v>0.44</v>
+        <v>0.86</v>
       </c>
       <c r="G17">
-        <v>-0.57</v>
+        <v>1.56</v>
       </c>
       <c r="H17">
-        <v>-0.82</v>
+        <v>-0.66</v>
       </c>
       <c r="I17">
         <v>50</v>
@@ -1527,19 +1527,19 @@
         <v>0.5</v>
       </c>
       <c r="K17">
-        <v>0.009714032867179714</v>
+        <v>0.2356468247517436</v>
       </c>
       <c r="L17">
-        <v>0.0762717342123974</v>
+        <v>0.4573410559117512</v>
       </c>
       <c r="M17" t="s">
         <v>120</v>
       </c>
       <c r="N17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O17">
-        <v>633.4</v>
+        <v>584.95</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1547,7 +1547,7 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18">
         <v>115</v>
@@ -1559,10 +1559,10 @@
         <v>50</v>
       </c>
       <c r="F18">
-        <v>0.77</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>-2.18</v>
+        <v>-2.42</v>
       </c>
       <c r="H18">
         <v>-2.94</v>
@@ -1574,10 +1574,10 @@
         <v>0.5</v>
       </c>
       <c r="K18">
-        <v>0.5289511071671765</v>
+        <v>1.983348539170497</v>
       </c>
       <c r="L18">
-        <v>0.67852768611175</v>
+        <v>1.846633723193622</v>
       </c>
       <c r="M18" t="s">
         <v>118</v>
@@ -1586,7 +1586,7 @@
         <v>5</v>
       </c>
       <c r="O18">
-        <v>69.39</v>
+        <v>69.34999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1600,19 +1600,19 @@
         <v>115</v>
       </c>
       <c r="D19">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E19">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="F19">
-        <v>-0.91</v>
+        <v>0.35</v>
       </c>
       <c r="G19">
-        <v>-1.98</v>
+        <v>-1.24</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="I19">
         <v>50</v>
@@ -1624,16 +1624,16 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>0.07123460823643463</v>
       </c>
       <c r="M19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O19">
-        <v>212.7</v>
+        <v>140.99</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1653,10 +1653,10 @@
         <v>40</v>
       </c>
       <c r="F20">
-        <v>0.5600000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="G20">
-        <v>-1.8</v>
+        <v>-1.9</v>
       </c>
       <c r="H20">
         <v>-2.38</v>
@@ -1668,10 +1668,10 @@
         <v>0.5</v>
       </c>
       <c r="K20">
-        <v>0.03783454823904283</v>
+        <v>0.1966981824298875</v>
       </c>
       <c r="L20">
-        <v>0.1078328097665582</v>
+        <v>0.3932104293404976</v>
       </c>
       <c r="M20" t="s">
         <v>118</v>
@@ -1688,7 +1688,7 @@
         <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C21">
         <v>110</v>
@@ -1700,13 +1700,13 @@
         <v>90</v>
       </c>
       <c r="F21">
-        <v>0.85</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="G21">
-        <v>0.98</v>
+        <v>-0.45</v>
       </c>
       <c r="H21">
-        <v>-0.12</v>
+        <v>-0.02</v>
       </c>
       <c r="I21">
         <v>50</v>
@@ -1715,10 +1715,10 @@
         <v>0.5</v>
       </c>
       <c r="K21">
-        <v>0.0168208578637526</v>
+        <v>0.4006731631614484</v>
       </c>
       <c r="L21">
-        <v>0.04357298474945534</v>
+        <v>0.7302916758504151</v>
       </c>
       <c r="M21" t="s">
         <v>120</v>
@@ -1727,7 +1727,7 @@
         <v>9</v>
       </c>
       <c r="O21">
-        <v>940.65</v>
+        <v>8671.5</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1735,7 +1735,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C22">
         <v>110</v>
@@ -1747,13 +1747,13 @@
         <v>90</v>
       </c>
       <c r="F22">
-        <v>0.44</v>
+        <v>0.77</v>
       </c>
       <c r="G22">
-        <v>-0.51</v>
+        <v>1.03</v>
       </c>
       <c r="H22">
-        <v>-0.02</v>
+        <v>-0.12</v>
       </c>
       <c r="I22">
         <v>50</v>
@@ -1762,10 +1762,10 @@
         <v>0.5</v>
       </c>
       <c r="K22">
-        <v>0.02154866100288385</v>
+        <v>0</v>
       </c>
       <c r="L22">
-        <v>0.210366126577746</v>
+        <v>0</v>
       </c>
       <c r="M22" t="s">
         <v>120</v>
@@ -1774,7 +1774,7 @@
         <v>9</v>
       </c>
       <c r="O22">
-        <v>8657</v>
+        <v>940.8</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1782,25 +1782,25 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C23">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D23">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="E23">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F23">
-        <v>-0.03</v>
+        <v>0.38</v>
       </c>
       <c r="G23">
-        <v>-4.21</v>
+        <v>-0.22</v>
       </c>
       <c r="H23">
-        <v>-5.1</v>
+        <v>0.3</v>
       </c>
       <c r="I23">
         <v>50</v>
@@ -1809,19 +1809,19 @@
         <v>0.5</v>
       </c>
       <c r="K23">
-        <v>0.1282916356307278</v>
+        <v>0.01935224612954743</v>
       </c>
       <c r="L23">
-        <v>0.1752873563218391</v>
+        <v>0.1565089105312109</v>
       </c>
       <c r="M23" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="N23">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O23">
-        <v>429.7</v>
+        <v>1885.7</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1829,25 +1829,25 @@
         <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D24">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="E24">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="F24">
-        <v>0.13</v>
+        <v>0.49</v>
       </c>
       <c r="G24">
-        <v>-0.07000000000000001</v>
+        <v>-4.6</v>
       </c>
       <c r="H24">
-        <v>0.14</v>
+        <v>-5.1</v>
       </c>
       <c r="I24">
         <v>50</v>
@@ -1856,19 +1856,19 @@
         <v>0.5</v>
       </c>
       <c r="K24">
-        <v>0.115420092830654</v>
+        <v>0</v>
       </c>
       <c r="L24">
-        <v>0.294760888918751</v>
+        <v>0.0009785214540828807</v>
       </c>
       <c r="M24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O24">
-        <v>138.51</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1876,7 +1876,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25">
         <v>100</v>
@@ -1888,10 +1888,10 @@
         <v>80</v>
       </c>
       <c r="F25">
-        <v>0.93</v>
+        <v>0.65</v>
       </c>
       <c r="G25">
-        <v>-0.46</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="H25">
         <v>-1.08</v>
@@ -1903,10 +1903,10 @@
         <v>0.5</v>
       </c>
       <c r="K25">
-        <v>0.04283861045473969</v>
+        <v>0.03751440046336296</v>
       </c>
       <c r="L25">
-        <v>0.3023116694440883</v>
+        <v>0.09650651017788374</v>
       </c>
       <c r="M25" t="s">
         <v>120</v>
@@ -1915,7 +1915,7 @@
         <v>8</v>
       </c>
       <c r="O25">
-        <v>919.45</v>
+        <v>918.95</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -1926,22 +1926,22 @@
         <v>107</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D26">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E26">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F26">
-        <v>0.19</v>
+        <v>0.09</v>
       </c>
       <c r="G26">
-        <v>-0.7</v>
+        <v>-1.03</v>
       </c>
       <c r="H26">
-        <v>-0.43</v>
+        <v>-0.55</v>
       </c>
       <c r="I26">
         <v>50</v>
@@ -1950,19 +1950,19 @@
         <v>0.5</v>
       </c>
       <c r="K26">
-        <v>0.1517177490539552</v>
+        <v>0.002556418354318414</v>
       </c>
       <c r="L26">
-        <v>0.3607347685146705</v>
+        <v>0.05455391415610097</v>
       </c>
       <c r="M26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O26">
-        <v>799.9</v>
+        <v>520</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1970,25 +1970,25 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C27">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E27">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F27">
-        <v>0.7</v>
+        <v>-0.02</v>
       </c>
       <c r="G27">
-        <v>0.01</v>
+        <v>-2.04</v>
       </c>
       <c r="H27">
-        <v>-0.17</v>
+        <v>-0.42</v>
       </c>
       <c r="I27">
         <v>50</v>
@@ -1997,19 +1997,19 @@
         <v>0.5</v>
       </c>
       <c r="K27">
-        <v>0.06508755385439707</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>0.1420959147424512</v>
+        <v>0.002520733029164881</v>
       </c>
       <c r="M27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N27">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O27">
-        <v>537.85</v>
+        <v>256.3</v>
       </c>
     </row>
     <row r="28" spans="1:15">
@@ -2017,7 +2017,7 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28">
         <v>95</v>
@@ -2029,13 +2029,13 @@
         <v>50</v>
       </c>
       <c r="F28">
-        <v>-0.13</v>
+        <v>1.27</v>
       </c>
       <c r="G28">
-        <v>-1.35</v>
+        <v>-2.26</v>
       </c>
       <c r="H28">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>50</v>
@@ -2044,10 +2044,10 @@
         <v>0.5</v>
       </c>
       <c r="K28">
-        <v>0.080287984137887</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>0.16606405962755</v>
+        <v>0</v>
       </c>
       <c r="M28" t="s">
         <v>119</v>
@@ -2056,7 +2056,7 @@
         <v>5</v>
       </c>
       <c r="O28">
-        <v>351.15</v>
+        <v>212.87</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2064,7 +2064,7 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C29">
         <v>95</v>
@@ -2076,13 +2076,13 @@
         <v>50</v>
       </c>
       <c r="F29">
-        <v>0.9399999999999999</v>
+        <v>0.11</v>
       </c>
       <c r="G29">
-        <v>-1.17</v>
+        <v>-1.35</v>
       </c>
       <c r="H29">
-        <v>-1.3</v>
+        <v>0.06</v>
       </c>
       <c r="I29">
         <v>50</v>
@@ -2091,10 +2091,10 @@
         <v>0.5</v>
       </c>
       <c r="K29">
-        <v>0.1197213855082675</v>
+        <v>0.02354250537280011</v>
       </c>
       <c r="L29">
-        <v>0.2096250950960026</v>
+        <v>0.06577526197687286</v>
       </c>
       <c r="M29" t="s">
         <v>119</v>
@@ -2103,7 +2103,7 @@
         <v>5</v>
       </c>
       <c r="O29">
-        <v>307.4</v>
+        <v>351.05</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2111,7 +2111,7 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30">
         <v>90</v>
@@ -2123,13 +2123,13 @@
         <v>70</v>
       </c>
       <c r="F30">
-        <v>0.27</v>
+        <v>0.5</v>
       </c>
       <c r="G30">
-        <v>1.88</v>
+        <v>-0.31</v>
       </c>
       <c r="H30">
-        <v>0.14</v>
+        <v>0.22</v>
       </c>
       <c r="I30">
         <v>50</v>
@@ -2138,10 +2138,10 @@
         <v>0.5</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>0.008485315535499863</v>
       </c>
       <c r="L30">
-        <v>0.04553170561451938</v>
+        <v>0.01849269387012672</v>
       </c>
       <c r="M30" t="s">
         <v>120</v>
@@ -2150,7 +2150,7 @@
         <v>7</v>
       </c>
       <c r="O30">
-        <v>51.94</v>
+        <v>1063.6</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2170,13 +2170,13 @@
         <v>70</v>
       </c>
       <c r="F31">
-        <v>-0.1</v>
+        <v>0.64</v>
       </c>
       <c r="G31">
-        <v>-0.37</v>
+        <v>-0.61</v>
       </c>
       <c r="H31">
-        <v>0.22</v>
+        <v>0.67</v>
       </c>
       <c r="I31">
         <v>50</v>
@@ -2185,10 +2185,10 @@
         <v>0.5</v>
       </c>
       <c r="K31">
-        <v>0.292226498582597</v>
+        <v>0</v>
       </c>
       <c r="L31">
-        <v>0.4549695012558306</v>
+        <v>0.1851570799817878</v>
       </c>
       <c r="M31" t="s">
         <v>120</v>
@@ -2197,7 +2197,7 @@
         <v>7</v>
       </c>
       <c r="O31">
-        <v>1061.9</v>
+        <v>604.2</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2205,25 +2205,25 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C32">
         <v>90</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E32">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F32">
-        <v>0.36</v>
+        <v>0.76</v>
       </c>
       <c r="G32">
-        <v>-0.26</v>
+        <v>-0.23</v>
       </c>
       <c r="H32">
-        <v>0.3</v>
+        <v>-0.17</v>
       </c>
       <c r="I32">
         <v>50</v>
@@ -2232,19 +2232,19 @@
         <v>0.5</v>
       </c>
       <c r="K32">
-        <v>0.9916763309965421</v>
+        <v>14.85636579976165</v>
       </c>
       <c r="L32">
-        <v>0.7977155277061632</v>
+        <v>11.25563425627817</v>
       </c>
       <c r="M32" t="s">
         <v>121</v>
       </c>
       <c r="N32">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O32">
-        <v>1885.4</v>
+        <v>536.65</v>
       </c>
     </row>
     <row r="33" spans="1:15">
@@ -2252,7 +2252,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33">
         <v>90</v>
@@ -2264,13 +2264,13 @@
         <v>70</v>
       </c>
       <c r="F33">
-        <v>0.61</v>
+        <v>0.5</v>
       </c>
       <c r="G33">
-        <v>-0.98</v>
+        <v>2.06</v>
       </c>
       <c r="H33">
-        <v>0.5600000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="I33">
         <v>50</v>
@@ -2279,10 +2279,10 @@
         <v>0.5</v>
       </c>
       <c r="K33">
-        <v>0.05011584951917541</v>
+        <v>0.06488773278831876</v>
       </c>
       <c r="L33">
-        <v>0.1088168801808591</v>
+        <v>0.05966461651684803</v>
       </c>
       <c r="M33" t="s">
         <v>120</v>
@@ -2291,7 +2291,7 @@
         <v>7</v>
       </c>
       <c r="O33">
-        <v>141.25</v>
+        <v>52.04</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2305,19 +2305,19 @@
         <v>85</v>
       </c>
       <c r="D34">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E34">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F34">
-        <v>-0.21</v>
+        <v>0.89</v>
       </c>
       <c r="G34">
-        <v>-1.82</v>
+        <v>-1.43</v>
       </c>
       <c r="H34">
-        <v>-0.42</v>
+        <v>-1.3</v>
       </c>
       <c r="I34">
         <v>50</v>
@@ -2326,19 +2326,19 @@
         <v>0.5</v>
       </c>
       <c r="K34">
-        <v>0.113219145281208</v>
+        <v>0.5791311163963189</v>
       </c>
       <c r="L34">
-        <v>0.3084892983036984</v>
+        <v>0.5879405885478606</v>
       </c>
       <c r="M34" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O34">
-        <v>256.7</v>
+        <v>306.9</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2346,7 +2346,7 @@
         <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C35">
         <v>85</v>
@@ -2358,13 +2358,13 @@
         <v>20</v>
       </c>
       <c r="F35">
-        <v>-1.12</v>
+        <v>1.12</v>
       </c>
       <c r="G35">
-        <v>-1.03</v>
+        <v>-2.58</v>
       </c>
       <c r="H35">
-        <v>0.54</v>
+        <v>-2.95</v>
       </c>
       <c r="I35">
         <v>50</v>
@@ -2373,10 +2373,10 @@
         <v>0.5</v>
       </c>
       <c r="K35">
-        <v>0.008131304301865955</v>
+        <v>1.674504670026542</v>
       </c>
       <c r="L35">
-        <v>0.03396162336559688</v>
+        <v>1.726023166023166</v>
       </c>
       <c r="M35" t="s">
         <v>118</v>
@@ -2385,7 +2385,7 @@
         <v>2</v>
       </c>
       <c r="O35">
-        <v>235.6</v>
+        <v>539</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2399,19 +2399,19 @@
         <v>85</v>
       </c>
       <c r="D36">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F36">
-        <v>0.37</v>
+        <v>0.47</v>
       </c>
       <c r="G36">
-        <v>-2.97</v>
+        <v>-1</v>
       </c>
       <c r="H36">
-        <v>-2.95</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I36">
         <v>50</v>
@@ -2420,19 +2420,19 @@
         <v>0.5</v>
       </c>
       <c r="K36">
-        <v>0.07714427596401495</v>
+        <v>0</v>
       </c>
       <c r="L36">
-        <v>0.2470734007730291</v>
+        <v>0.02240617414576461</v>
       </c>
       <c r="M36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="N36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O36">
-        <v>536.15</v>
+        <v>419</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2440,25 +2440,25 @@
         <v>50</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C37">
         <v>80</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F37">
-        <v>-0.02</v>
+        <v>0.34</v>
       </c>
       <c r="G37">
-        <v>0.02</v>
+        <v>-0.63</v>
       </c>
       <c r="H37">
-        <v>0.31</v>
+        <v>-0.43</v>
       </c>
       <c r="I37">
         <v>50</v>
@@ -2467,19 +2467,19 @@
         <v>0.5</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>1.293983323530441</v>
       </c>
       <c r="L37">
-        <v>0.5391120507399577</v>
+        <v>1.109463067339068</v>
       </c>
       <c r="M37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N37">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="O37">
-        <v>261.35</v>
+        <v>800.25</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2487,7 +2487,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C38">
         <v>80</v>
@@ -2499,13 +2499,13 @@
         <v>60</v>
       </c>
       <c r="F38">
-        <v>0.29</v>
+        <v>0.48</v>
       </c>
       <c r="G38">
-        <v>-0.82</v>
+        <v>-0.76</v>
       </c>
       <c r="H38">
-        <v>0.4</v>
+        <v>-0.24</v>
       </c>
       <c r="I38">
         <v>50</v>
@@ -2514,10 +2514,10 @@
         <v>0.5</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>0.2543637661410725</v>
       </c>
       <c r="L38">
-        <v>0</v>
+        <v>0.2225755166931637</v>
       </c>
       <c r="M38" t="s">
         <v>120</v>
@@ -2526,7 +2526,7 @@
         <v>6</v>
       </c>
       <c r="O38">
-        <v>31550</v>
+        <v>697.85</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2534,25 +2534,25 @@
         <v>52</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C39">
         <v>80</v>
       </c>
       <c r="D39">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F39">
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="G39">
-        <v>-0.53</v>
+        <v>-0.2</v>
       </c>
       <c r="H39">
-        <v>0.67</v>
+        <v>0.14</v>
       </c>
       <c r="I39">
         <v>50</v>
@@ -2561,19 +2561,19 @@
         <v>0.5</v>
       </c>
       <c r="K39">
-        <v>0.6724437146846811</v>
+        <v>1.541057489193308</v>
       </c>
       <c r="L39">
-        <v>0.92152466367713</v>
+        <v>1.090127035657482</v>
       </c>
       <c r="M39" t="s">
         <v>121</v>
       </c>
       <c r="N39">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O39">
-        <v>603.7</v>
+        <v>138.61</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2581,7 +2581,7 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C40">
         <v>80</v>
@@ -2593,13 +2593,13 @@
         <v>60</v>
       </c>
       <c r="F40">
-        <v>0.29</v>
+        <v>0.15</v>
       </c>
       <c r="G40">
-        <v>-0.9399999999999999</v>
+        <v>0.44</v>
       </c>
       <c r="H40">
-        <v>-0.24</v>
+        <v>0.31</v>
       </c>
       <c r="I40">
         <v>50</v>
@@ -2608,10 +2608,10 @@
         <v>0.5</v>
       </c>
       <c r="K40">
-        <v>0.05342891037128881</v>
+        <v>0</v>
       </c>
       <c r="L40">
-        <v>0.1655498620417816</v>
+        <v>0.003409478349812479</v>
       </c>
       <c r="M40" t="s">
         <v>120</v>
@@ -2620,7 +2620,7 @@
         <v>6</v>
       </c>
       <c r="O40">
-        <v>697.2</v>
+        <v>260.7</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2640,10 +2640,10 @@
         <v>30</v>
       </c>
       <c r="F41">
-        <v>1.02</v>
+        <v>0.97</v>
       </c>
       <c r="G41">
-        <v>-1.7</v>
+        <v>-1.73</v>
       </c>
       <c r="H41">
         <v>0.31</v>
@@ -2655,10 +2655,10 @@
         <v>0.5</v>
       </c>
       <c r="K41">
-        <v>0.4119313853935583</v>
+        <v>0.04473748547607041</v>
       </c>
       <c r="L41">
-        <v>0.6681657565049791</v>
+        <v>0.1386691666178395</v>
       </c>
       <c r="M41" t="s">
         <v>119</v>
@@ -2667,7 +2667,7 @@
         <v>3</v>
       </c>
       <c r="O41">
-        <v>2238.8</v>
+        <v>2237.5</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2675,25 +2675,25 @@
         <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C42">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D42">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E42">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="F42">
-        <v>0.06</v>
+        <v>0.27</v>
       </c>
       <c r="G42">
-        <v>-1.26</v>
+        <v>-0.11</v>
       </c>
       <c r="H42">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
       <c r="I42">
         <v>50</v>
@@ -2702,19 +2702,19 @@
         <v>0.5</v>
       </c>
       <c r="K42">
-        <v>0</v>
+        <v>0.05627647952250012</v>
       </c>
       <c r="L42">
-        <v>0</v>
+        <v>0.2660753880266075</v>
       </c>
       <c r="M42" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N42">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O42">
-        <v>1523</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2734,10 +2734,10 @@
         <v>50</v>
       </c>
       <c r="F43">
-        <v>0.09</v>
+        <v>0.48</v>
       </c>
       <c r="G43">
-        <v>0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H43">
         <v>-0.46</v>
@@ -2749,10 +2749,10 @@
         <v>0.5</v>
       </c>
       <c r="K43">
-        <v>0.002910048858186053</v>
+        <v>0</v>
       </c>
       <c r="L43">
-        <v>0.1007156109196926</v>
+        <v>0.1544607190412783</v>
       </c>
       <c r="M43" t="s">
         <v>120</v>
@@ -2761,7 +2761,7 @@
         <v>5</v>
       </c>
       <c r="O43">
-        <v>3182.2</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -2769,25 +2769,25 @@
         <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C44">
         <v>70</v>
       </c>
       <c r="D44">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E44">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F44">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="G44">
-        <v>0.59</v>
+        <v>-0.14</v>
       </c>
       <c r="H44">
-        <v>-0.23</v>
+        <v>0.4</v>
       </c>
       <c r="I44">
         <v>50</v>
@@ -2796,19 +2796,19 @@
         <v>0.5</v>
       </c>
       <c r="K44">
-        <v>0.0004238620187840083</v>
+        <v>1.925501432664756</v>
       </c>
       <c r="L44">
-        <v>0.005009601736661935</v>
+        <v>2.957746478873239</v>
       </c>
       <c r="M44" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O44">
-        <v>349.15</v>
+        <v>31755</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -2816,25 +2816,25 @@
         <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C45">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D45">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="E45">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F45">
-        <v>0.52</v>
+        <v>1.1</v>
       </c>
       <c r="G45">
-        <v>-1.03</v>
+        <v>0.61</v>
       </c>
       <c r="H45">
-        <v>-0.95</v>
+        <v>-0.23</v>
       </c>
       <c r="I45">
         <v>50</v>
@@ -2843,19 +2843,19 @@
         <v>0.5</v>
       </c>
       <c r="K45">
-        <v>0.01023297617178457</v>
+        <v>0</v>
       </c>
       <c r="L45">
-        <v>0.01924516198011333</v>
+        <v>0</v>
       </c>
       <c r="M45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N45">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O45">
-        <v>2263.4</v>
+        <v>349.2</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -2875,13 +2875,13 @@
         <v>20</v>
       </c>
       <c r="F46">
-        <v>0.01</v>
+        <v>1.1</v>
       </c>
       <c r="G46">
-        <v>-2.11</v>
+        <v>-1.01</v>
       </c>
       <c r="H46">
-        <v>-1.44</v>
+        <v>-1.48</v>
       </c>
       <c r="I46">
         <v>50</v>
@@ -2890,10 +2890,10 @@
         <v>0.5</v>
       </c>
       <c r="K46">
-        <v>0.08130216750237844</v>
+        <v>0.08779210239950394</v>
       </c>
       <c r="L46">
-        <v>0.4574428196475441</v>
+        <v>0.2644942411997321</v>
       </c>
       <c r="M46" t="s">
         <v>119</v>
@@ -2902,7 +2902,7 @@
         <v>2</v>
       </c>
       <c r="O46">
-        <v>4433.6</v>
+        <v>798.75</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -2910,7 +2910,7 @@
         <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C47">
         <v>65</v>
@@ -2922,13 +2922,13 @@
         <v>20</v>
       </c>
       <c r="F47">
-        <v>0.5</v>
+        <v>0.23</v>
       </c>
       <c r="G47">
-        <v>-1.25</v>
+        <v>-1.11</v>
       </c>
       <c r="H47">
-        <v>0.06</v>
+        <v>-0.77</v>
       </c>
       <c r="I47">
         <v>50</v>
@@ -2937,10 +2937,10 @@
         <v>0.5</v>
       </c>
       <c r="K47">
-        <v>0.3533152749971261</v>
+        <v>0.05650686981473015</v>
       </c>
       <c r="L47">
-        <v>0.5756987402356979</v>
+        <v>0.1270319733017548</v>
       </c>
       <c r="M47" t="s">
         <v>119</v>
@@ -2949,7 +2949,7 @@
         <v>2</v>
       </c>
       <c r="O47">
-        <v>771.55</v>
+        <v>1154.9</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -2957,26 +2957,26 @@
         <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C48">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E48">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F48">
+        <v>0.54</v>
+      </c>
+      <c r="G48">
+        <v>-1.26</v>
+      </c>
+      <c r="H48">
         <v>0.06</v>
       </c>
-      <c r="G48">
-        <v>-0.17</v>
-      </c>
-      <c r="H48">
-        <v>0.05</v>
-      </c>
       <c r="I48">
         <v>50</v>
       </c>
@@ -2984,19 +2984,19 @@
         <v>0.5</v>
       </c>
       <c r="K48">
-        <v>0</v>
+        <v>0.04445169594460995</v>
       </c>
       <c r="L48">
-        <v>0</v>
+        <v>0.2631353021978022</v>
       </c>
       <c r="M48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N48">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O48">
-        <v>646.7</v>
+        <v>772.05</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -3004,25 +3004,25 @@
         <v>62</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C49">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D49">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="E49">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F49">
-        <v>0.39</v>
+        <v>0.37</v>
       </c>
       <c r="G49">
-        <v>-0.17</v>
+        <v>-1.36</v>
       </c>
       <c r="H49">
-        <v>0.05</v>
+        <v>-0.95</v>
       </c>
       <c r="I49">
         <v>50</v>
@@ -3031,19 +3031,19 @@
         <v>0.5</v>
       </c>
       <c r="K49">
-        <v>0.2603308098558667</v>
+        <v>0.08178485978095675</v>
       </c>
       <c r="L49">
-        <v>0.7013868521389367</v>
+        <v>0.6178396072013094</v>
       </c>
       <c r="M49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O49">
-        <v>1923</v>
+        <v>2260.2</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -3051,25 +3051,25 @@
         <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50">
         <v>60</v>
       </c>
       <c r="D50">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E50">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F50">
-        <v>0.42</v>
+        <v>0.77</v>
       </c>
       <c r="G50">
-        <v>0.25</v>
+        <v>-0.76</v>
       </c>
       <c r="H50">
-        <v>0.44</v>
+        <v>-0.87</v>
       </c>
       <c r="I50">
         <v>50</v>
@@ -3078,19 +3078,19 @@
         <v>0.5</v>
       </c>
       <c r="K50">
-        <v>4.3553835662062</v>
+        <v>0.04792066467736799</v>
       </c>
       <c r="L50">
-        <v>3.104927837732415</v>
+        <v>0.04012334212579411</v>
       </c>
       <c r="M50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O50">
-        <v>1545</v>
+        <v>28.63</v>
       </c>
     </row>
     <row r="51" spans="1:15">
@@ -3098,7 +3098,7 @@
         <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C51">
         <v>60</v>
@@ -3110,13 +3110,13 @@
         <v>40</v>
       </c>
       <c r="F51">
-        <v>0.73</v>
+        <v>0.28</v>
       </c>
       <c r="G51">
-        <v>-0.65</v>
+        <v>-0.37</v>
       </c>
       <c r="H51">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="I51">
         <v>50</v>
@@ -3137,7 +3137,7 @@
         <v>4</v>
       </c>
       <c r="O51">
-        <v>420.75</v>
+        <v>647.5</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3145,7 +3145,7 @@
         <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52">
         <v>60</v>
@@ -3157,13 +3157,13 @@
         <v>40</v>
       </c>
       <c r="F52">
-        <v>0.45</v>
+        <v>0.66</v>
       </c>
       <c r="G52">
-        <v>0.35</v>
+        <v>-0.05</v>
       </c>
       <c r="H52">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="I52">
         <v>50</v>
@@ -3172,10 +3172,10 @@
         <v>0.5</v>
       </c>
       <c r="K52">
-        <v>0.08843036109066167</v>
+        <v>0.06640344241483619</v>
       </c>
       <c r="L52">
-        <v>0.3065134099616859</v>
+        <v>0.2668202904702708</v>
       </c>
       <c r="M52" t="s">
         <v>120</v>
@@ -3184,7 +3184,7 @@
         <v>4</v>
       </c>
       <c r="O52">
-        <v>424.8</v>
+        <v>1925.5</v>
       </c>
     </row>
     <row r="53" spans="1:15">
@@ -3192,7 +3192,7 @@
         <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C53">
         <v>55</v>
@@ -3204,13 +3204,13 @@
         <v>10</v>
       </c>
       <c r="F53">
-        <v>0.65</v>
+        <v>0.51</v>
       </c>
       <c r="G53">
-        <v>-1.89</v>
+        <v>-1.38</v>
       </c>
       <c r="H53">
-        <v>-1.08</v>
+        <v>-1</v>
       </c>
       <c r="I53">
         <v>50</v>
@@ -3219,10 +3219,10 @@
         <v>0.5</v>
       </c>
       <c r="K53">
-        <v>0.01075872483681201</v>
+        <v>0</v>
       </c>
       <c r="L53">
-        <v>0.383569286561127</v>
+        <v>0.017319909301849</v>
       </c>
       <c r="M53" t="s">
         <v>119</v>
@@ -3231,7 +3231,7 @@
         <v>1</v>
       </c>
       <c r="O53">
-        <v>624</v>
+        <v>506.55</v>
       </c>
     </row>
     <row r="54" spans="1:15">
@@ -3245,19 +3245,19 @@
         <v>55</v>
       </c>
       <c r="D54">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E54">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F54">
-        <v>-0.3</v>
+        <v>0.53</v>
       </c>
       <c r="G54">
-        <v>-1.16</v>
+        <v>-1.66</v>
       </c>
       <c r="H54">
-        <v>-0.77</v>
+        <v>-1.44</v>
       </c>
       <c r="I54">
         <v>50</v>
@@ -3266,19 +3266,19 @@
         <v>0.5</v>
       </c>
       <c r="K54">
-        <v>0.04942244453311508</v>
+        <v>0.6571834389773118</v>
       </c>
       <c r="L54">
-        <v>0.2036993060502916</v>
+        <v>0.8125819134993447</v>
       </c>
       <c r="M54" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O54">
-        <v>1154</v>
+        <v>4454.7</v>
       </c>
     </row>
     <row r="55" spans="1:15">
@@ -3286,7 +3286,7 @@
         <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C55">
         <v>55</v>
@@ -3298,13 +3298,13 @@
         <v>10</v>
       </c>
       <c r="F55">
-        <v>0.27</v>
+        <v>0.88</v>
       </c>
       <c r="G55">
-        <v>-1.57</v>
+        <v>-1.91</v>
       </c>
       <c r="H55">
-        <v>-1</v>
+        <v>-1.08</v>
       </c>
       <c r="I55">
         <v>50</v>
@@ -3313,10 +3313,10 @@
         <v>0.5</v>
       </c>
       <c r="K55">
-        <v>0.04696309694735256</v>
+        <v>0.6663671253571122</v>
       </c>
       <c r="L55">
-        <v>0.1110626807881941</v>
+        <v>2.374482027560952</v>
       </c>
       <c r="M55" t="s">
         <v>119</v>
@@ -3325,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="O55">
-        <v>505.85</v>
+        <v>625</v>
       </c>
     </row>
     <row r="56" spans="1:15">
@@ -3333,7 +3333,7 @@
         <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56">
         <v>50</v>
@@ -3345,13 +3345,13 @@
         <v>30</v>
       </c>
       <c r="F56">
-        <v>0.21</v>
+        <v>1.66</v>
       </c>
       <c r="G56">
-        <v>-0.34</v>
+        <v>4.61</v>
       </c>
       <c r="H56">
-        <v>-0.73</v>
+        <v>3.19</v>
       </c>
       <c r="I56">
         <v>50</v>
@@ -3360,10 +3360,10 @@
         <v>0.5</v>
       </c>
       <c r="K56">
-        <v>0.02555910543130824</v>
+        <v>0.1041038210600044</v>
       </c>
       <c r="L56">
-        <v>0.03831417624521073</v>
+        <v>0.3784452760126877</v>
       </c>
       <c r="M56" t="s">
         <v>120</v>
@@ -3372,7 +3372,7 @@
         <v>3</v>
       </c>
       <c r="O56">
-        <v>3023.6</v>
+        <v>265.7</v>
       </c>
     </row>
     <row r="57" spans="1:15">
@@ -3380,7 +3380,7 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -3392,13 +3392,13 @@
         <v>30</v>
       </c>
       <c r="F57">
-        <v>1.1</v>
+        <v>0.59</v>
       </c>
       <c r="G57">
-        <v>-0.1</v>
+        <v>-1</v>
       </c>
       <c r="H57">
-        <v>-0.31</v>
+        <v>0.18</v>
       </c>
       <c r="I57">
         <v>50</v>
@@ -3410,7 +3410,7 @@
         <v>0</v>
       </c>
       <c r="L57">
-        <v>0.04301075268817205</v>
+        <v>0.005377789728421619</v>
       </c>
       <c r="M57" t="s">
         <v>120</v>
@@ -3419,7 +3419,7 @@
         <v>3</v>
       </c>
       <c r="O57">
-        <v>44180</v>
+        <v>1527.1</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -3427,7 +3427,7 @@
         <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C58">
         <v>50</v>
@@ -3439,13 +3439,13 @@
         <v>30</v>
       </c>
       <c r="F58">
-        <v>0.58</v>
+        <v>0.77</v>
       </c>
       <c r="G58">
-        <v>-0.83</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H58">
-        <v>0.05</v>
+        <v>-0.2</v>
       </c>
       <c r="I58">
         <v>50</v>
@@ -3454,10 +3454,10 @@
         <v>0.5</v>
       </c>
       <c r="K58">
-        <v>0.07855217558726435</v>
+        <v>0</v>
       </c>
       <c r="L58">
-        <v>0.7039337474120083</v>
+        <v>0</v>
       </c>
       <c r="M58" t="s">
         <v>120</v>
@@ -3466,7 +3466,7 @@
         <v>3</v>
       </c>
       <c r="O58">
-        <v>1043.6</v>
+        <v>5155.5</v>
       </c>
     </row>
     <row r="59" spans="1:15">
@@ -3474,25 +3474,25 @@
         <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C59">
         <v>50</v>
       </c>
       <c r="D59">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E59">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F59">
-        <v>0.44</v>
+        <v>0.72</v>
       </c>
       <c r="G59">
-        <v>-0.93</v>
+        <v>-0.25</v>
       </c>
       <c r="H59">
-        <v>-0.55</v>
+        <v>-1.29</v>
       </c>
       <c r="I59">
         <v>50</v>
@@ -3501,19 +3501,19 @@
         <v>0.5</v>
       </c>
       <c r="K59">
-        <v>1.071015749169217</v>
+        <v>0</v>
       </c>
       <c r="L59">
-        <v>2.676161851380503</v>
+        <v>0</v>
       </c>
       <c r="M59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N59">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O59">
-        <v>520.5</v>
+        <v>323.3</v>
       </c>
     </row>
     <row r="60" spans="1:15">
@@ -3521,7 +3521,7 @@
         <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C60">
         <v>50</v>
@@ -3533,13 +3533,13 @@
         <v>30</v>
       </c>
       <c r="F60">
-        <v>1.22</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="G60">
-        <v>0.95</v>
+        <v>-0.68</v>
       </c>
       <c r="H60">
-        <v>-0.2</v>
+        <v>-0.73</v>
       </c>
       <c r="I60">
         <v>50</v>
@@ -3551,7 +3551,7 @@
         <v>0</v>
       </c>
       <c r="L60">
-        <v>0</v>
+        <v>0.03891050583657588</v>
       </c>
       <c r="M60" t="s">
         <v>120</v>
@@ -3560,7 +3560,7 @@
         <v>3</v>
       </c>
       <c r="O60">
-        <v>5158</v>
+        <v>3017.4</v>
       </c>
     </row>
     <row r="61" spans="1:15">
@@ -3568,7 +3568,7 @@
         <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C61">
         <v>50</v>
@@ -3580,13 +3580,13 @@
         <v>30</v>
       </c>
       <c r="F61">
-        <v>1.5</v>
+        <v>0.99</v>
       </c>
       <c r="G61">
-        <v>5.23</v>
+        <v>-1</v>
       </c>
       <c r="H61">
-        <v>3.19</v>
+        <v>0.05</v>
       </c>
       <c r="I61">
         <v>50</v>
@@ -3595,10 +3595,10 @@
         <v>0.5</v>
       </c>
       <c r="K61">
-        <v>0.2125297067627207</v>
+        <v>0</v>
       </c>
       <c r="L61">
-        <v>0.501999146496195</v>
+        <v>0</v>
       </c>
       <c r="M61" t="s">
         <v>120</v>
@@ -3607,7 +3607,7 @@
         <v>3</v>
       </c>
       <c r="O61">
-        <v>264.7</v>
+        <v>1044.3</v>
       </c>
     </row>
     <row r="62" spans="1:15">
@@ -3615,7 +3615,7 @@
         <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C62">
         <v>50</v>
@@ -3627,13 +3627,13 @@
         <v>30</v>
       </c>
       <c r="F62">
-        <v>1.38</v>
+        <v>1.28</v>
       </c>
       <c r="G62">
-        <v>0.03</v>
+        <v>-0.17</v>
       </c>
       <c r="H62">
-        <v>-0.41</v>
+        <v>-0.31</v>
       </c>
       <c r="I62">
         <v>50</v>
@@ -3642,10 +3642,10 @@
         <v>0.5</v>
       </c>
       <c r="K62">
-        <v>0.3066711639688767</v>
+        <v>0.01492537313432836</v>
       </c>
       <c r="L62">
-        <v>0.6803715264431708</v>
+        <v>0.1574803149606299</v>
       </c>
       <c r="M62" t="s">
         <v>120</v>
@@ -3654,7 +3654,7 @@
         <v>3</v>
       </c>
       <c r="O62">
-        <v>751.55</v>
+        <v>44245</v>
       </c>
     </row>
     <row r="63" spans="1:15">
@@ -3662,7 +3662,7 @@
         <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C63">
         <v>50</v>
@@ -3677,10 +3677,10 @@
         <v>0.82</v>
       </c>
       <c r="G63">
-        <v>0.88</v>
+        <v>-0.65</v>
       </c>
       <c r="H63">
-        <v>-0.83</v>
+        <v>0.36</v>
       </c>
       <c r="I63">
         <v>50</v>
@@ -3692,7 +3692,7 @@
         <v>0</v>
       </c>
       <c r="L63">
-        <v>0</v>
+        <v>0.9013821192495159</v>
       </c>
       <c r="M63" t="s">
         <v>120</v>
@@ -3701,7 +3701,7 @@
         <v>3</v>
       </c>
       <c r="O63">
-        <v>929</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -3709,7 +3709,7 @@
         <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C64">
         <v>50</v>
@@ -3721,13 +3721,13 @@
         <v>30</v>
       </c>
       <c r="F64">
-        <v>0.93</v>
+        <v>0.7</v>
       </c>
       <c r="G64">
-        <v>-0.66</v>
+        <v>0.59</v>
       </c>
       <c r="H64">
-        <v>0.36</v>
+        <v>-0.83</v>
       </c>
       <c r="I64">
         <v>50</v>
@@ -3739,7 +3739,7 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <v>0.0149852021129135</v>
+        <v>0</v>
       </c>
       <c r="M64" t="s">
         <v>120</v>
@@ -3748,7 +3748,7 @@
         <v>3</v>
       </c>
       <c r="O64">
-        <v>61.58</v>
+        <v>926.8</v>
       </c>
     </row>
     <row r="65" spans="1:15">
@@ -3768,10 +3768,10 @@
         <v>30</v>
       </c>
       <c r="F65">
-        <v>0.08</v>
+        <v>0.67</v>
       </c>
       <c r="G65">
-        <v>0.29</v>
+        <v>0.32</v>
       </c>
       <c r="H65">
         <v>-0.01</v>
@@ -3783,10 +3783,10 @@
         <v>0.5</v>
       </c>
       <c r="K65">
-        <v>0.3296146044622012</v>
+        <v>0.01866977829637959</v>
       </c>
       <c r="L65">
-        <v>0.9767092411720512</v>
+        <v>0.08136696501220504</v>
       </c>
       <c r="M65" t="s">
         <v>120</v>
@@ -3795,7 +3795,7 @@
         <v>3</v>
       </c>
       <c r="O65">
-        <v>101.7</v>
+        <v>101.64</v>
       </c>
     </row>
     <row r="66" spans="1:15">
@@ -3803,25 +3803,25 @@
         <v>79</v>
       </c>
       <c r="B66" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C66">
+        <v>50</v>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+      <c r="E66">
         <v>40</v>
       </c>
-      <c r="D66">
-        <v>20</v>
-      </c>
-      <c r="E66">
-        <v>20</v>
-      </c>
       <c r="F66">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
       <c r="G66">
-        <v>-0.42</v>
+        <v>0.12</v>
       </c>
       <c r="H66">
-        <v>-0.23</v>
+        <v>0.02</v>
       </c>
       <c r="I66">
         <v>50</v>
@@ -3830,19 +3830,19 @@
         <v>0.5</v>
       </c>
       <c r="K66">
-        <v>0.1123869528387191</v>
+        <v>0.7715624138881254</v>
       </c>
       <c r="L66">
-        <v>0.3121843282505171</v>
+        <v>0.408997955010225</v>
       </c>
       <c r="M66" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N66">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O66">
-        <v>310.05</v>
+        <v>424.3</v>
       </c>
     </row>
     <row r="67" spans="1:15">
@@ -3850,25 +3850,25 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C67">
         <v>40</v>
       </c>
       <c r="D67">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E67">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F67">
-        <v>1.06</v>
+        <v>1.65</v>
       </c>
       <c r="G67">
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="H67">
-        <v>-0.39</v>
+        <v>-0.41</v>
       </c>
       <c r="I67">
         <v>50</v>
@@ -3877,19 +3877,19 @@
         <v>0.5</v>
       </c>
       <c r="K67">
-        <v>0.1713056301954048</v>
+        <v>1.340396545634404</v>
       </c>
       <c r="L67">
-        <v>0.4107311112255015</v>
+        <v>1.52732655627751</v>
       </c>
       <c r="M67" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N67">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O67">
-        <v>1459.7</v>
+        <v>752.35</v>
       </c>
     </row>
     <row r="68" spans="1:15">
@@ -3897,7 +3897,7 @@
         <v>81</v>
       </c>
       <c r="B68" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C68">
         <v>40</v>
@@ -3909,13 +3909,13 @@
         <v>20</v>
       </c>
       <c r="F68">
-        <v>0.8100000000000001</v>
+        <v>-0.03</v>
       </c>
       <c r="G68">
-        <v>-0.32</v>
+        <v>-0.11</v>
       </c>
       <c r="H68">
-        <v>-1.29</v>
+        <v>-0.24</v>
       </c>
       <c r="I68">
         <v>50</v>
@@ -3924,10 +3924,10 @@
         <v>0.5</v>
       </c>
       <c r="K68">
-        <v>0.2278586686964265</v>
+        <v>0.4052040746239994</v>
       </c>
       <c r="L68">
-        <v>0.9670696123384743</v>
+        <v>0.7651382687965776</v>
       </c>
       <c r="M68" t="s">
         <v>120</v>
@@ -3936,7 +3936,7 @@
         <v>2</v>
       </c>
       <c r="O68">
-        <v>323.6</v>
+        <v>1400.5</v>
       </c>
     </row>
     <row r="69" spans="1:15">
@@ -3944,25 +3944,25 @@
         <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C69">
         <v>40</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E69">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F69">
-        <v>0.63</v>
+        <v>0.29</v>
       </c>
       <c r="G69">
-        <v>-0.73</v>
+        <v>-0.91</v>
       </c>
       <c r="H69">
-        <v>-0.87</v>
+        <v>0.54</v>
       </c>
       <c r="I69">
         <v>50</v>
@@ -3971,19 +3971,19 @@
         <v>0.5</v>
       </c>
       <c r="K69">
-        <v>0.9417161125541519</v>
+        <v>0.2181485674475825</v>
       </c>
       <c r="L69">
-        <v>0.9156333412170153</v>
+        <v>1.361968193557156</v>
       </c>
       <c r="M69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N69">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O69">
-        <v>28.6</v>
+        <v>235</v>
       </c>
     </row>
     <row r="70" spans="1:15">
@@ -3991,7 +3991,7 @@
         <v>83</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C70">
         <v>40</v>
@@ -4003,13 +4003,13 @@
         <v>20</v>
       </c>
       <c r="F70">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
       <c r="G70">
-        <v>0.25</v>
+        <v>-0.48</v>
       </c>
       <c r="H70">
-        <v>-0.74</v>
+        <v>-0.23</v>
       </c>
       <c r="I70">
         <v>50</v>
@@ -4018,10 +4018,10 @@
         <v>0.5</v>
       </c>
       <c r="K70">
-        <v>0.0158941120398279</v>
+        <v>0.3804185351269371</v>
       </c>
       <c r="L70">
-        <v>0.550665599767222</v>
+        <v>0.8665120337071478</v>
       </c>
       <c r="M70" t="s">
         <v>120</v>
@@ -4030,7 +4030,7 @@
         <v>2</v>
       </c>
       <c r="O70">
-        <v>199.95</v>
+        <v>310.15</v>
       </c>
     </row>
     <row r="71" spans="1:15">
@@ -4038,7 +4038,7 @@
         <v>84</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="C71">
         <v>40</v>
@@ -4050,13 +4050,13 @@
         <v>20</v>
       </c>
       <c r="F71">
-        <v>-0.02</v>
+        <v>1.28</v>
       </c>
       <c r="G71">
-        <v>-0.02</v>
+        <v>0.24</v>
       </c>
       <c r="H71">
-        <v>-0.24</v>
+        <v>0.32</v>
       </c>
       <c r="I71">
         <v>50</v>
@@ -4065,10 +4065,10 @@
         <v>0.5</v>
       </c>
       <c r="K71">
-        <v>0.01689280410424901</v>
+        <v>0</v>
       </c>
       <c r="L71">
-        <v>0.1471371822715129</v>
+        <v>0.0002606440514511358</v>
       </c>
       <c r="M71" t="s">
         <v>120</v>
@@ -4077,7 +4077,7 @@
         <v>2</v>
       </c>
       <c r="O71">
-        <v>1401.7</v>
+        <v>517.1</v>
       </c>
     </row>
     <row r="72" spans="1:15">
@@ -4085,25 +4085,25 @@
         <v>85</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C72">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D72">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E72">
         <v>20</v>
       </c>
       <c r="F72">
-        <v>1.06</v>
+        <v>0.63</v>
       </c>
       <c r="G72">
-        <v>-0.93</v>
+        <v>0.36</v>
       </c>
       <c r="H72">
-        <v>-1.48</v>
+        <v>-0.39</v>
       </c>
       <c r="I72">
         <v>50</v>
@@ -4112,19 +4112,19 @@
         <v>0.5</v>
       </c>
       <c r="K72">
-        <v>0.02384690833794674</v>
+        <v>0.6506053451902091</v>
       </c>
       <c r="L72">
-        <v>0.2443159731699046</v>
+        <v>0.5511750941092685</v>
       </c>
       <c r="M72" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N72">
         <v>2</v>
       </c>
       <c r="O72">
-        <v>797.5</v>
+        <v>1460.6</v>
       </c>
     </row>
     <row r="73" spans="1:15">
@@ -4132,25 +4132,25 @@
         <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C73">
         <v>30</v>
       </c>
       <c r="D73">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E73">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F73">
-        <v>0.49</v>
+        <v>0.8</v>
       </c>
       <c r="G73">
-        <v>-0.36</v>
+        <v>1.71</v>
       </c>
       <c r="H73">
-        <v>-0.71</v>
+        <v>0.78</v>
       </c>
       <c r="I73">
         <v>50</v>
@@ -4159,19 +4159,19 @@
         <v>0.5</v>
       </c>
       <c r="K73">
-        <v>0.01558734150686493</v>
+        <v>4.849932718372999</v>
       </c>
       <c r="L73">
-        <v>0.05176022835394862</v>
+        <v>3.039644077222531</v>
       </c>
       <c r="M73" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N73">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O73">
-        <v>863.9</v>
+        <v>1092.4</v>
       </c>
     </row>
     <row r="74" spans="1:15">
@@ -4179,7 +4179,7 @@
         <v>87</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C74">
         <v>30</v>
@@ -4191,13 +4191,13 @@
         <v>10</v>
       </c>
       <c r="F74">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
       <c r="G74">
-        <v>0.21</v>
+        <v>1.11</v>
       </c>
       <c r="H74">
-        <v>-0.86</v>
+        <v>-0.17</v>
       </c>
       <c r="I74">
         <v>50</v>
@@ -4206,10 +4206,10 @@
         <v>0.5</v>
       </c>
       <c r="K74">
-        <v>0.01453023630994929</v>
+        <v>0</v>
       </c>
       <c r="L74">
-        <v>0.05212774736610459</v>
+        <v>0</v>
       </c>
       <c r="M74" t="s">
         <v>120</v>
@@ -4218,7 +4218,7 @@
         <v>1</v>
       </c>
       <c r="O74">
-        <v>426.8</v>
+        <v>1131.4</v>
       </c>
     </row>
     <row r="75" spans="1:15">
@@ -4226,7 +4226,7 @@
         <v>88</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C75">
         <v>30</v>
@@ -4238,13 +4238,13 @@
         <v>10</v>
       </c>
       <c r="F75">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>-0.28</v>
+        <v>0.6</v>
       </c>
       <c r="H75">
-        <v>-0.58</v>
+        <v>-0.93</v>
       </c>
       <c r="I75">
         <v>50</v>
@@ -4253,10 +4253,10 @@
         <v>0.5</v>
       </c>
       <c r="K75">
-        <v>0</v>
+        <v>0.2402029300616236</v>
       </c>
       <c r="L75">
-        <v>0.08361204013377926</v>
+        <v>0.1856594110115237</v>
       </c>
       <c r="M75" t="s">
         <v>120</v>
@@ -4265,7 +4265,7 @@
         <v>1</v>
       </c>
       <c r="O75">
-        <v>147.42</v>
+        <v>250.7</v>
       </c>
     </row>
     <row r="76" spans="1:15">
@@ -4273,7 +4273,7 @@
         <v>89</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C76">
         <v>30</v>
@@ -4285,13 +4285,13 @@
         <v>10</v>
       </c>
       <c r="F76">
-        <v>0.16</v>
+        <v>-0.43</v>
       </c>
       <c r="G76">
-        <v>1.01</v>
+        <v>-0.44</v>
       </c>
       <c r="H76">
-        <v>-0.93</v>
+        <v>-1.6</v>
       </c>
       <c r="I76">
         <v>50</v>
@@ -4300,10 +4300,10 @@
         <v>0.5</v>
       </c>
       <c r="K76">
-        <v>0.0001395907200088924</v>
+        <v>0.4302257315885546</v>
       </c>
       <c r="L76">
-        <v>0.0008483922965979468</v>
+        <v>0.6635975507847517</v>
       </c>
       <c r="M76" t="s">
         <v>120</v>
@@ -4312,7 +4312,7 @@
         <v>1</v>
       </c>
       <c r="O76">
-        <v>250.85</v>
+        <v>958.2</v>
       </c>
     </row>
     <row r="77" spans="1:15">
@@ -4320,7 +4320,7 @@
         <v>90</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C77">
         <v>30</v>
@@ -4332,13 +4332,13 @@
         <v>10</v>
       </c>
       <c r="F77">
-        <v>0.86</v>
+        <v>0.64</v>
       </c>
       <c r="G77">
-        <v>0.43</v>
+        <v>1.09</v>
       </c>
       <c r="H77">
-        <v>-0.22</v>
+        <v>0.25</v>
       </c>
       <c r="I77">
         <v>50</v>
@@ -4359,7 +4359,7 @@
         <v>1</v>
       </c>
       <c r="O77">
-        <v>200.84</v>
+        <v>8381</v>
       </c>
     </row>
     <row r="78" spans="1:15">
@@ -4367,7 +4367,7 @@
         <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C78">
         <v>30</v>
@@ -4382,10 +4382,10 @@
         <v>0.9</v>
       </c>
       <c r="G78">
-        <v>1.66</v>
+        <v>-0.03</v>
       </c>
       <c r="H78">
-        <v>-0.12</v>
+        <v>-0.71</v>
       </c>
       <c r="I78">
         <v>50</v>
@@ -4394,10 +4394,10 @@
         <v>0.5</v>
       </c>
       <c r="K78">
-        <v>0.1309210085414235</v>
+        <v>0.02092967782146614</v>
       </c>
       <c r="L78">
-        <v>0.1657180385288967</v>
+        <v>0.05754908598510495</v>
       </c>
       <c r="M78" t="s">
         <v>120</v>
@@ -4406,7 +4406,7 @@
         <v>1</v>
       </c>
       <c r="O78">
-        <v>42.77</v>
+        <v>868</v>
       </c>
     </row>
     <row r="79" spans="1:15">
@@ -4414,25 +4414,25 @@
         <v>92</v>
       </c>
       <c r="B79" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C79">
         <v>30</v>
       </c>
       <c r="D79">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E79">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F79">
-        <v>0.38</v>
+        <v>1.01</v>
       </c>
       <c r="G79">
-        <v>-0.02</v>
+        <v>-0.2</v>
       </c>
       <c r="H79">
-        <v>0.32</v>
+        <v>-0.74</v>
       </c>
       <c r="I79">
         <v>50</v>
@@ -4441,19 +4441,19 @@
         <v>0.5</v>
       </c>
       <c r="K79">
-        <v>0.1228450821557568</v>
+        <v>16.83879343927486</v>
       </c>
       <c r="L79">
-        <v>0.1871229841191678</v>
+        <v>14.42663916544366</v>
       </c>
       <c r="M79" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N79">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O79">
-        <v>515.3</v>
+        <v>199.5</v>
       </c>
     </row>
     <row r="80" spans="1:15">
@@ -4461,7 +4461,7 @@
         <v>93</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C80">
         <v>30</v>
@@ -4473,13 +4473,13 @@
         <v>10</v>
       </c>
       <c r="F80">
-        <v>0.79</v>
+        <v>1.63</v>
       </c>
       <c r="G80">
-        <v>0.27</v>
+        <v>-0.26</v>
       </c>
       <c r="H80">
-        <v>-0.5</v>
+        <v>-0.78</v>
       </c>
       <c r="I80">
         <v>50</v>
@@ -4488,10 +4488,10 @@
         <v>0.5</v>
       </c>
       <c r="K80">
-        <v>0</v>
+        <v>0.01643646408840172</v>
       </c>
       <c r="L80">
-        <v>0</v>
+        <v>0.1483605535469393</v>
       </c>
       <c r="M80" t="s">
         <v>120</v>
@@ -4500,7 +4500,7 @@
         <v>1</v>
       </c>
       <c r="O80">
-        <v>1305.3</v>
+        <v>371.55</v>
       </c>
     </row>
     <row r="81" spans="1:15">
@@ -4508,7 +4508,7 @@
         <v>94</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C81">
         <v>30</v>
@@ -4520,14 +4520,14 @@
         <v>10</v>
       </c>
       <c r="F81">
-        <v>1.1</v>
+        <v>0.29</v>
       </c>
       <c r="G81">
+        <v>-0.15</v>
+      </c>
+      <c r="H81">
         <v>-0.11</v>
       </c>
-      <c r="H81">
-        <v>0.27</v>
-      </c>
       <c r="I81">
         <v>50</v>
       </c>
@@ -4535,10 +4535,10 @@
         <v>0.5</v>
       </c>
       <c r="K81">
-        <v>0.2933618182769744</v>
+        <v>0.1434626671014056</v>
       </c>
       <c r="L81">
-        <v>0.4414718150507538</v>
+        <v>0.09216589861751152</v>
       </c>
       <c r="M81" t="s">
         <v>120</v>
@@ -4547,7 +4547,7 @@
         <v>1</v>
       </c>
       <c r="O81">
-        <v>95.09</v>
+        <v>1853.1</v>
       </c>
     </row>
     <row r="82" spans="1:15">
@@ -4555,7 +4555,7 @@
         <v>95</v>
       </c>
       <c r="B82" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C82">
         <v>30</v>
@@ -4567,13 +4567,13 @@
         <v>10</v>
       </c>
       <c r="F82">
-        <v>1.45</v>
+        <v>0.4</v>
       </c>
       <c r="G82">
-        <v>1.4</v>
+        <v>-0.23</v>
       </c>
       <c r="H82">
-        <v>-0.17</v>
+        <v>-0.59</v>
       </c>
       <c r="I82">
         <v>50</v>
@@ -4582,10 +4582,10 @@
         <v>0.5</v>
       </c>
       <c r="K82">
-        <v>0.0200411511637196</v>
+        <v>0</v>
       </c>
       <c r="L82">
-        <v>0.1267812769410213</v>
+        <v>0.03218760777100816</v>
       </c>
       <c r="M82" t="s">
         <v>120</v>
@@ -4594,7 +4594,7 @@
         <v>1</v>
       </c>
       <c r="O82">
-        <v>1133.2</v>
+        <v>571.95</v>
       </c>
     </row>
     <row r="83" spans="1:15">
@@ -4602,7 +4602,7 @@
         <v>96</v>
       </c>
       <c r="B83" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C83">
         <v>30</v>
@@ -4614,13 +4614,13 @@
         <v>10</v>
       </c>
       <c r="F83">
-        <v>1.49</v>
+        <v>0.82</v>
       </c>
       <c r="G83">
-        <v>-0.16</v>
+        <v>0.02</v>
       </c>
       <c r="H83">
-        <v>-0.78</v>
+        <v>-0.4</v>
       </c>
       <c r="I83">
         <v>50</v>
@@ -4629,10 +4629,10 @@
         <v>0.5</v>
       </c>
       <c r="K83">
-        <v>0.03989208142184743</v>
+        <v>0.02535423560473994</v>
       </c>
       <c r="L83">
-        <v>0.3986153362005664</v>
+        <v>0.157013043209495</v>
       </c>
       <c r="M83" t="s">
         <v>120</v>
@@ -4641,7 +4641,7 @@
         <v>1</v>
       </c>
       <c r="O83">
-        <v>371.3</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="84" spans="1:15">
@@ -4661,13 +4661,13 @@
         <v>10</v>
       </c>
       <c r="F84">
-        <v>0.99</v>
+        <v>0.86</v>
       </c>
       <c r="G84">
-        <v>-0.03</v>
+        <v>-0.12</v>
       </c>
       <c r="H84">
-        <v>-0.6899999999999999</v>
+        <v>-0.58</v>
       </c>
       <c r="I84">
         <v>50</v>
@@ -4676,10 +4676,10 @@
         <v>0.5</v>
       </c>
       <c r="K84">
-        <v>0.01035451520785949</v>
+        <v>0</v>
       </c>
       <c r="L84">
-        <v>0.2159443309885788</v>
+        <v>0</v>
       </c>
       <c r="M84" t="s">
         <v>120</v>
@@ -4688,7 +4688,7 @@
         <v>1</v>
       </c>
       <c r="O84">
-        <v>79.59</v>
+        <v>147.4</v>
       </c>
     </row>
     <row r="85" spans="1:15">
@@ -4696,7 +4696,7 @@
         <v>98</v>
       </c>
       <c r="B85" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C85">
         <v>30</v>
@@ -4708,13 +4708,13 @@
         <v>10</v>
       </c>
       <c r="F85">
-        <v>0.87</v>
+        <v>0.95</v>
       </c>
       <c r="G85">
-        <v>-0.27</v>
+        <v>0.55</v>
       </c>
       <c r="H85">
-        <v>0.25</v>
+        <v>-0.22</v>
       </c>
       <c r="I85">
         <v>50</v>
@@ -4723,10 +4723,10 @@
         <v>0.5</v>
       </c>
       <c r="K85">
-        <v>0.09578107183580388</v>
+        <v>0</v>
       </c>
       <c r="L85">
-        <v>0.4827586206896552</v>
+        <v>0</v>
       </c>
       <c r="M85" t="s">
         <v>120</v>
@@ -4735,7 +4735,7 @@
         <v>1</v>
       </c>
       <c r="O85">
-        <v>8392</v>
+        <v>200.79</v>
       </c>
     </row>
     <row r="86" spans="1:15">
@@ -4743,7 +4743,7 @@
         <v>99</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C86">
         <v>30</v>
@@ -4755,13 +4755,13 @@
         <v>10</v>
       </c>
       <c r="F86">
-        <v>0.46</v>
+        <v>1.34</v>
       </c>
       <c r="G86">
-        <v>0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="H86">
-        <v>-0.36</v>
+        <v>-0.86</v>
       </c>
       <c r="I86">
         <v>50</v>
@@ -4770,10 +4770,10 @@
         <v>0.5</v>
       </c>
       <c r="K86">
-        <v>0.1545846304844734</v>
+        <v>0.00661758070606945</v>
       </c>
       <c r="L86">
-        <v>0.19638786603542</v>
+        <v>0.04383731485376492</v>
       </c>
       <c r="M86" t="s">
         <v>120</v>
@@ -4782,7 +4782,7 @@
         <v>1</v>
       </c>
       <c r="O86">
-        <v>522.05</v>
+        <v>426.6</v>
       </c>
     </row>
     <row r="87" spans="1:15">
@@ -4790,7 +4790,7 @@
         <v>100</v>
       </c>
       <c r="B87" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C87">
         <v>30</v>
@@ -4802,13 +4802,13 @@
         <v>10</v>
       </c>
       <c r="F87">
-        <v>0.59</v>
+        <v>0.8</v>
       </c>
       <c r="G87">
-        <v>-0.37</v>
+        <v>-0.1</v>
       </c>
       <c r="H87">
-        <v>-0.59</v>
+        <v>-0.36</v>
       </c>
       <c r="I87">
         <v>50</v>
@@ -4829,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="O87">
-        <v>571.7</v>
+        <v>522</v>
       </c>
     </row>
     <row r="88" spans="1:15">
@@ -4837,7 +4837,7 @@
         <v>101</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C88">
         <v>30</v>
@@ -4849,10 +4849,10 @@
         <v>10</v>
       </c>
       <c r="F88">
-        <v>1.16</v>
+        <v>1.36</v>
       </c>
       <c r="G88">
-        <v>2</v>
+        <v>1.97</v>
       </c>
       <c r="H88">
         <v>0.15</v>
@@ -4864,10 +4864,10 @@
         <v>0.5</v>
       </c>
       <c r="K88">
-        <v>0.05933023898907978</v>
+        <v>0</v>
       </c>
       <c r="L88">
-        <v>0.162546467087874</v>
+        <v>0.08925355213127877</v>
       </c>
       <c r="M88" t="s">
         <v>120</v>
@@ -4876,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="O88">
-        <v>387.8</v>
+        <v>387.9</v>
       </c>
     </row>
     <row r="89" spans="1:15">
@@ -4884,25 +4884,25 @@
         <v>102</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C89">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D89">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E89">
         <v>10</v>
       </c>
       <c r="F89">
-        <v>0.3</v>
+        <v>0.59</v>
       </c>
       <c r="G89">
-        <v>-0.21</v>
+        <v>0.45</v>
       </c>
       <c r="H89">
-        <v>-0.4</v>
+        <v>-0.12</v>
       </c>
       <c r="I89">
         <v>50</v>
@@ -4911,19 +4911,19 @@
         <v>0.5</v>
       </c>
       <c r="K89">
-        <v>0.05559371338532978</v>
+        <v>0.6300391058755539</v>
       </c>
       <c r="L89">
-        <v>0.1277955271565495</v>
+        <v>0.6628874462832587</v>
       </c>
       <c r="M89" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N89">
         <v>1</v>
       </c>
       <c r="O89">
-        <v>1386.4</v>
+        <v>42.62</v>
       </c>
     </row>
     <row r="90" spans="1:15">
@@ -4931,7 +4931,7 @@
         <v>103</v>
       </c>
       <c r="B90" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C90">
         <v>20</v>
@@ -4943,13 +4943,13 @@
         <v>10</v>
       </c>
       <c r="F90">
-        <v>0.12</v>
+        <v>1.1</v>
       </c>
       <c r="G90">
-        <v>1.15</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="H90">
-        <v>0.78</v>
+        <v>-0.5</v>
       </c>
       <c r="I90">
         <v>50</v>
@@ -4958,10 +4958,10 @@
         <v>0.5</v>
       </c>
       <c r="K90">
-        <v>2.791676920132349</v>
+        <v>2.816010124980238</v>
       </c>
       <c r="L90">
-        <v>3.658187029738445</v>
+        <v>2.314694408322497</v>
       </c>
       <c r="M90" t="s">
         <v>121</v>
@@ -4970,7 +4970,7 @@
         <v>1</v>
       </c>
       <c r="O90">
-        <v>1086.6</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="91" spans="1:15">
@@ -4978,25 +4978,25 @@
         <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C91">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D91">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>10</v>
       </c>
       <c r="F91">
-        <v>0.58</v>
+        <v>1.2</v>
       </c>
       <c r="G91">
-        <v>-0.15</v>
+        <v>-0.13</v>
       </c>
       <c r="H91">
-        <v>-0.11</v>
+        <v>0.27</v>
       </c>
       <c r="I91">
         <v>50</v>
@@ -5005,10 +5005,10 @@
         <v>0.5</v>
       </c>
       <c r="K91">
-        <v>4.411469821535933</v>
+        <v>1.172428035760128</v>
       </c>
       <c r="L91">
-        <v>5.269461077844311</v>
+        <v>1.041164902666991</v>
       </c>
       <c r="M91" t="s">
         <v>121</v>
@@ -5017,7 +5017,7 @@
         <v>1</v>
       </c>
       <c r="O91">
-        <v>1853.1</v>
+        <v>95.16</v>
       </c>
     </row>
     <row r="92" spans="1:15">
@@ -5025,7 +5025,7 @@
         <v>105</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C92">
         <v>10</v>
@@ -5037,13 +5037,13 @@
         <v>10</v>
       </c>
       <c r="F92">
-        <v>-0.47</v>
+        <v>1.12</v>
       </c>
       <c r="G92">
-        <v>-0.53</v>
+        <v>0.37</v>
       </c>
       <c r="H92">
-        <v>-1.6</v>
+        <v>-0.6899999999999999</v>
       </c>
       <c r="I92">
         <v>50</v>
@@ -5052,10 +5052,10 @@
         <v>0.5</v>
       </c>
       <c r="K92">
-        <v>0.9200183274488589</v>
+        <v>0.9200928381962777</v>
       </c>
       <c r="L92">
-        <v>0.6647480710182532</v>
+        <v>0.9078640657588026</v>
       </c>
       <c r="M92" t="s">
         <v>121</v>
@@ -5064,7 +5064,7 @@
         <v>1</v>
       </c>
       <c r="O92">
-        <v>957.4</v>
+        <v>79.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>